<commit_message>
Now support keyboard, mouse and joystick When open the camera, this device change to tetris mode automatically
</commit_message>
<xml_diff>
--- a/trunk/SuperJoystick/Tetris/Resource.xlsx
+++ b/trunk/SuperJoystick/Tetris/Resource.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BattaryIcon" sheetId="2" r:id="rId1"/>
     <sheet name="StringResource" sheetId="3" r:id="rId2"/>
     <sheet name="ClockFace" sheetId="4" r:id="rId3"/>
     <sheet name="SuperJoystick" sheetId="5" r:id="rId4"/>
+    <sheet name="Array" sheetId="6" r:id="rId5"/>
+    <sheet name="Power" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="184">
   <si>
     <t>/**</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -732,7 +734,28 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1040,7 +1063,7 @@
   <dimension ref="A1:AC53"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AG74" sqref="AG74"/>
+      <selection activeCell="AA49" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3635,7 +3658,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="V1:X1048576 Y1:Y11 Y13:Y1048576 U13 A3:U12 A14:U33 A36:U51 A54:U1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3743,27 +3766,27 @@
         <v>164</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f t="shared" ref="F3:F56" si="0">CONCATENATE("#define   ",A3,"         ")</f>
+        <f t="shared" ref="F3:F8" si="0">CONCATENATE("#define   ",A3,"         ")</f>
         <v xml:space="preserve">#define   STR_CAMERA_OFF         </v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G57" si="1">B3</f>
+        <f t="shared" ref="G3:G8" si="1">B3</f>
         <v>1</v>
       </c>
       <c r="I3" s="7" t="str">
-        <f t="shared" ref="I3:I59" si="2">IF(EXACT($A3,"STR_LAST"),"};",CONCATENATE("  [",$A3,"]"))</f>
+        <f t="shared" ref="I3:I57" si="2">IF(EXACT($A3,"STR_LAST"),"};",CONCATENATE("  [",$A3,"]"))</f>
         <v xml:space="preserve">  [STR_CAMERA_OFF]</v>
       </c>
       <c r="J3" s="7" t="str">
-        <f t="shared" ref="J3:J59" si="3">IF(EXACT($A3,"STR_LAST"),"",CONCATENATE("= ","""",$C3,""","))</f>
+        <f t="shared" ref="J3:J57" si="3">IF(EXACT($A3,"STR_LAST"),"",CONCATENATE("= ","""",$C3,""","))</f>
         <v>= "Camera Off",</v>
       </c>
       <c r="L3" s="8" t="str">
-        <f t="shared" ref="L3:L59" si="4">IF(EXACT($A3,"STR_LAST"),"};",CONCATENATE("  [",$A3,"]"))</f>
+        <f t="shared" ref="L3:L57" si="4">IF(EXACT($A3,"STR_LAST"),"};",CONCATENATE("  [",$A3,"]"))</f>
         <v xml:space="preserve">  [STR_CAMERA_OFF]</v>
       </c>
       <c r="M3" s="8" t="str">
-        <f t="shared" ref="M3:M59" si="5">IF(EXACT($A3,"STR_LAST"),"",CONCATENATE("= ","""",$D3,""","))</f>
+        <f t="shared" ref="M3:M57" si="5">IF(EXACT($A3,"STR_LAST"),"",CONCATENATE("= ","""",$D3,""","))</f>
         <v>= "摄像头关",</v>
       </c>
     </row>
@@ -8514,7 +8537,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="AL1:BE13 AK14:BE32 BF24:BG30 BF1:BJ23 AI1:AJ32 AI33:AI53 E46:J62 K46:AB53 AI56:AI64 BM1:DN71 BH24:BK64 E36:AB44 A1:AB34 A36:D62 AC1:AH53 AJ33:BE64 AI65:BL71 BF34:BG64 K56:AH71 BM69:BQ131 A63:J131 B68:BL131 BU69:BU131 H42:L51">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8527,7 +8550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -8912,4 +8935,4820 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC69"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="AA53" sqref="AA53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="2.375" customWidth="1"/>
+    <col min="2" max="25" width="2.25" customWidth="1"/>
+    <col min="27" max="27" width="12.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="C2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" s="3">
+        <f>A3+A4*2+A5*4+A6*8+A7*16+A8*32+A9*64+A10*128</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:L15" si="0">B3+B4*2+B5*4+B6*8+B7*16+B8*32+B9*64+B10*128</f>
+        <v>32</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="3">
+        <f>A11+A12*2+A13*4+A14*8</f>
+        <v>0</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16:L16" si="1">B11+B12*2+B13*4+B14*8</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="C21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="3">
+        <f>A22+A23*2+A24*4+A25*8+A26*16+A27*32+A28*64+A29*128</f>
+        <v>0</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" ref="B34:L34" si="2">B22+B23*2+B24*4+B25*8+B26*16+B27*32+B28*64+B29*128</f>
+        <v>32</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="2"/>
+        <v>248</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="3">
+        <f>A30+A31*2+A32*4+A33*8</f>
+        <v>0</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" ref="B35:L35" si="3">B30+B31*2+B32*4+B33*8</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="C39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" s="3">
+        <f>A40+A41*2+A42*4+A43*8+A44*16+A45*32+A46*64+A47*128</f>
+        <v>0</v>
+      </c>
+      <c r="B52" s="3">
+        <f t="shared" ref="B52:L52" si="4">B40+B41*2+B42*4+B43*8+B44*16+B45*32+B46*64+B47*128</f>
+        <v>64</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="4"/>
+        <v>254</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="J52" s="3">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="K52" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L52" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="3">
+        <f>A48+A49*2+A50*4+A51*8</f>
+        <v>0</v>
+      </c>
+      <c r="B53" s="3">
+        <f t="shared" ref="B53:L53" si="5">B48+B49*2+B50*4+B51*8</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="3">
+        <f>A56+A57*2+A58*4+A59*8+A60*16+A61*32+A62*64+A63*128</f>
+        <v>0</v>
+      </c>
+      <c r="B68" s="3">
+        <f t="shared" ref="B68:L68" si="6">B56+B57*2+B58*4+B59*8+B60*16+B61*32+B62*64+B63*128</f>
+        <v>32</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="6"/>
+        <v>112</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="6"/>
+        <v>248</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="6"/>
+        <v>172</v>
+      </c>
+      <c r="F68" s="3">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+      <c r="G68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="H68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="J68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="K68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="L68" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="3">
+        <f>A64+A65*2+A66*4+A67*8</f>
+        <v>0</v>
+      </c>
+      <c r="B69" s="3">
+        <f t="shared" ref="B69:L69" si="7">B64+B65*2+B66*4+B67*8</f>
+        <v>0</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="G69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="C21:Q21"/>
+    <mergeCell ref="C39:Q39"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="V1:X1048576 Y1:Y11 Y13:Y1048576 U13 A36:U51 A3:U12 A13:L14 A14:U33 A22:L35 A40:L53 A54:U1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:L53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="2.375" customWidth="1"/>
+    <col min="2" max="25" width="2.25" customWidth="1"/>
+    <col min="27" max="27" width="12.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="C2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" s="3">
+        <f>A3+A4*2+A5*4+A6*8+A7*16+A8*32+A9*64+A10*128</f>
+        <v>112</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:L15" si="0">B3+B4*2+B5*4+B6*8+B7*16+B8*32+B9*64+B10*128</f>
+        <v>140</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>241</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="3">
+        <f>A11+A12*2+A13*4+A14*8</f>
+        <v>0</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16:L16" si="1">B11+B12*2+B13*4+B14*8</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="C21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="3">
+        <f>A22+A23*2+A24*4+A25*8+A26*16+A27*32+A28*64+A29*128</f>
+        <v>112</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" ref="B34:L34" si="2">B22+B23*2+B24*4+B25*8+B26*16+B27*32+B28*64+B29*128</f>
+        <v>140</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="3">
+        <f>A30+A31*2+A32*4+A33*8</f>
+        <v>0</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" ref="B35:L35" si="3">B30+B31*2+B32*4+B33*8</f>
+        <v>1</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="C39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" s="3">
+        <f>A40+A41*2+A42*4+A43*8+A44*16+A45*32+A46*64+A47*128</f>
+        <v>112</v>
+      </c>
+      <c r="B52" s="3">
+        <f t="shared" ref="B52:L52" si="4">B40+B41*2+B42*4+B43*8+B44*16+B45*32+B46*64+B47*128</f>
+        <v>140</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="4"/>
+        <v>129</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="4"/>
+        <v>129</v>
+      </c>
+      <c r="H52" s="3">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J52" s="3">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+      <c r="K52" s="3">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+      <c r="L52" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="3">
+        <f>A48+A49*2+A50*4+A51*8</f>
+        <v>0</v>
+      </c>
+      <c r="B53" s="3">
+        <f t="shared" ref="B53:L53" si="5">B48+B49*2+B50*4+B51*8</f>
+        <v>1</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J53" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K53" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="3">
+        <f>A56+A57*2+A58*4+A59*8+A60*16+A61*32+A62*64+A63*128</f>
+        <v>0</v>
+      </c>
+      <c r="B68" s="3">
+        <f t="shared" ref="B68:L68" si="6">B56+B57*2+B58*4+B59*8+B60*16+B61*32+B62*64+B63*128</f>
+        <v>32</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="6"/>
+        <v>112</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="6"/>
+        <v>248</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="6"/>
+        <v>172</v>
+      </c>
+      <c r="F68" s="3">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+      <c r="G68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="H68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="J68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="K68" s="3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="L68" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="3">
+        <f>A64+A65*2+A66*4+A67*8</f>
+        <v>0</v>
+      </c>
+      <c r="B69" s="3">
+        <f t="shared" ref="B69:L69" si="7">B64+B65*2+B66*4+B67*8</f>
+        <v>0</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="G69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="C21:Q21"/>
+    <mergeCell ref="C39:Q39"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="V1:X1048576 Y1:Y11 Y13:Y1048576 U13 A36:U51 A3:U12 M14:U33 A54:U1048576 A13:L35 A40:L53">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1. Add air mouse function 2. Use ctrl + array to simulate the arrow key directly in keyboard mode 3. Fix the bug of AD sampling
</commit_message>
<xml_diff>
--- a/trunk/SuperJoystick/Tetris/Resource.xlsx
+++ b/trunk/SuperJoystick/Tetris/Resource.xlsx
@@ -734,7 +734,14 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3658,7 +3665,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="V1:X1048576 Y1:Y11 Y13:Y1048576 U13 A3:U12 A14:U33 A36:U51 A54:U1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8537,7 +8544,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="AL1:BE13 AK14:BE32 BF24:BG30 BF1:BJ23 AI1:AJ32 AI33:AI53 E46:J62 K46:AB53 AI56:AI64 BM1:DN71 BH24:BK64 E36:AB44 A1:AB34 A36:D62 AC1:AH53 AJ33:BE64 AI65:BL71 BF34:BG64 K56:AH71 BM69:BQ131 A63:J131 B68:BL131 BU69:BU131 H42:L51">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11337,7 +11344,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="V1:X1048576 Y1:Y11 Y13:Y1048576 U13 A36:U51 A3:U12 A13:L14 A14:U33 A22:L35 A40:L53 A54:U1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11349,8 +11356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:L53"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC63" sqref="AC63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -13186,10 +13193,10 @@
         <v>0</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -13221,22 +13228,22 @@
     </row>
     <row r="57" spans="1:21">
       <c r="A57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -13259,19 +13266,19 @@
     </row>
     <row r="58" spans="1:21">
       <c r="A58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -13300,16 +13307,16 @@
         <v>0</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -13341,10 +13348,10 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -13376,34 +13383,34 @@
         <v>0</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -13417,10 +13424,10 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -13458,10 +13465,10 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -13499,7 +13506,7 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -13540,7 +13547,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -13640,47 +13647,47 @@
     <row r="68" spans="1:12">
       <c r="A68" s="3">
         <f>A56+A57*2+A58*4+A59*8+A60*16+A61*32+A62*64+A63*128</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B68" s="3">
         <f t="shared" ref="B68:L68" si="6">B56+B57*2+B58*4+B59*8+B60*16+B61*32+B62*64+B63*128</f>
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C68" s="3">
         <f t="shared" si="6"/>
-        <v>112</v>
+        <v>15</v>
       </c>
       <c r="D68" s="3">
         <f t="shared" si="6"/>
-        <v>248</v>
+        <v>6</v>
       </c>
       <c r="E68" s="3">
         <f t="shared" si="6"/>
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="F68" s="3">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="G68" s="3">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="H68" s="3">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I68" s="3">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="J68" s="3">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K68" s="3">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="L68" s="3">
         <f t="shared" si="6"/>
@@ -13706,11 +13713,11 @@
       </c>
       <c r="E69" s="3">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="3">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G69" s="3">
         <f t="shared" si="7"/>
@@ -13744,8 +13751,8 @@
     <mergeCell ref="C39:Q39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="V1:X1048576 Y1:Y11 Y13:Y1048576 U13 A36:U51 A3:U12 M14:U33 A54:U1048576 A13:L35 A40:L53">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="V1:X1048576 Y1:Y11 Y13:Y1048576 U13 A36:U51 A3:U12 M14:U33 A13:L35 A40:L53 A54:U1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>